<commit_message>
update to use `nexial.scope.required.variables`
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/web-stuff/artifact/data/BrowserMeta.data.xlsx
+++ b/examples/web-stuff/artifact/data/BrowserMeta.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/examples/web-stuff/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEB62AF-9676-E349-9AFC-43B8E7616151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92606A2C-1CC6-1242-95C0-3A96DA169BB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="-21140" windowWidth="19200" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6280" yWindow="-21140" windowWidth="12800" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>true</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>css=[data-object=browser] &gt; .subrows &gt; [data-object=version] &gt; span</t>
+  </si>
+  <si>
+    <t>nexial.scope.required.variables</t>
+  </si>
+  <si>
+    <t>homepage.url</t>
+  </si>
+  <si>
+    <t>https://userstack.com</t>
   </si>
 </sst>
 </file>
@@ -289,7 +298,86 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -974,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA197"/>
+  <dimension ref="A1:AAA185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1010,168 +1098,184 @@
     </row>
     <row r="3" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="HA3" s="3"/>
       <c r="AAA3" s="3"/>
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="HA4" s="6"/>
-      <c r="AAA4" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="HA4" s="3"/>
+      <c r="AAA4" s="3"/>
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="HA5" s="6"/>
       <c r="AAA5" s="7"/>
     </row>
     <row r="6" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="HA6" s="6"/>
       <c r="AAA6" s="7"/>
     </row>
     <row r="7" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="HA7" s="6"/>
       <c r="AAA7" s="7"/>
     </row>
     <row r="8" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="HA8" s="6"/>
+      <c r="AAA8" s="7"/>
     </row>
     <row r="9" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -1633,152 +1737,138 @@
     <row r="185" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
     </row>
-    <row r="186" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="1"/>
-    </row>
-    <row r="187" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="1"/>
-    </row>
-    <row r="188" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="1"/>
-    </row>
-    <row r="189" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="1"/>
-    </row>
-    <row r="190" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="1"/>
-    </row>
-    <row r="191" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="1"/>
-    </row>
-    <row r="192" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="1"/>
-    </row>
-    <row r="193" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="1"/>
-    </row>
-    <row r="194" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="1"/>
-    </row>
-    <row r="195" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="1"/>
-    </row>
-    <row r="196" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="1"/>
-    </row>
-    <row r="197" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="1"/>
-    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
-  <conditionalFormatting sqref="A1:A9 A11:A12 A19:A1048576 A14">
-    <cfRule type="beginsWith" dxfId="29" priority="31" stopIfTrue="1" operator="beginsWith" text="//">
+  <conditionalFormatting sqref="A1:A2 A12:A13 A15 A18:A1048576 A4:A10">
+    <cfRule type="beginsWith" dxfId="35" priority="37" stopIfTrue="1" operator="beginsWith" text="//">
       <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="28" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="34" priority="38" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="27" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="33" priority="39" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="26" priority="34" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="40" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:AZ1048576 B1:AZ9 C10:AZ10 B11:AZ12 B14:AZ14 C13:AZ13 C15:AZ18">
-    <cfRule type="expression" dxfId="25" priority="35" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:AZ2 C11:AZ11 B12:AZ13 B15:AZ15 C14:AZ14 C16:AZ17 B18:AZ1048576 B4:AZ10 C3:AZ3">
+    <cfRule type="expression" dxfId="31" priority="41" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="24" priority="38">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="44">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
+  <conditionalFormatting sqref="A11">
+    <cfRule type="beginsWith" dxfId="29" priority="25" stopIfTrue="1" operator="beginsWith" text="//">
+      <formula>LEFT(A11,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="28" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A11,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="27" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A11,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="26" priority="28" stopIfTrue="1">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="24" priority="30">
+      <formula>LEN(TRIM(B11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
     <cfRule type="beginsWith" dxfId="23" priority="19" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A10,LEN("//"))="//"</formula>
+      <formula>LEFT(A14,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="22" priority="20" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A10,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="21" priority="21" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A10,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="20" priority="22" stopIfTrue="1">
-      <formula>LEN(TRIM(A10))&gt;0</formula>
+      <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10">
+  <conditionalFormatting sqref="B14">
     <cfRule type="expression" dxfId="19" priority="23" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="18" priority="24">
-      <formula>LEN(TRIM(B10))&gt;0</formula>
+      <formula>LEN(TRIM(B14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
+  <conditionalFormatting sqref="A16">
     <cfRule type="beginsWith" dxfId="17" priority="13" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A13,LEN("//"))="//"</formula>
+      <formula>LEFT(A16,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="16" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="15" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="14" priority="16" stopIfTrue="1">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
+      <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
+  <conditionalFormatting sqref="B16">
     <cfRule type="expression" dxfId="13" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="12" priority="18">
-      <formula>LEN(TRIM(B13))&gt;0</formula>
+      <formula>LEN(TRIM(B16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
+  <conditionalFormatting sqref="A17">
     <cfRule type="beginsWith" dxfId="11" priority="7" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A15,LEN("//"))="//"</formula>
+      <formula>LEFT(A17,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="10" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A17,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="9" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A17,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="8" priority="10" stopIfTrue="1">
-      <formula>LEN(TRIM(A15))&gt;0</formula>
+      <formula>LEN(TRIM(A17))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
+  <conditionalFormatting sqref="B17">
     <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="6" priority="12">
-      <formula>LEN(TRIM(B15))&gt;0</formula>
+      <formula>LEN(TRIM(B17))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
+  <conditionalFormatting sqref="A3">
     <cfRule type="beginsWith" dxfId="5" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A16,LEN("//"))="//"</formula>
+      <formula>LEFT(A3,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="4" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A3,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="3" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A3,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="2" priority="4" stopIfTrue="1">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
+      <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
+  <conditionalFormatting sqref="B3">
     <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="6">
-      <formula>LEN(TRIM(B16))&gt;0</formula>
+      <formula>LEN(TRIM(B3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>